<commit_message>
Update information and add custom profile sheet
</commit_message>
<xml_diff>
--- a/conversations.xlsx
+++ b/conversations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngduc\PycharmProjects\conversations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653B88B3-3247-441D-815B-38CDEC91D584}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B84ADD-DB32-44A5-8C3A-673666AE5BD2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="859">
   <si>
     <t>customer</t>
   </si>
@@ -2664,6 +2664,54 @@
   </si>
   <si>
     <t xml:space="preserve">Motivations </t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>xe đẩy, máy hút sữa,bình sữa</t>
+  </si>
+  <si>
+    <t>Không có hướng dẫn sử dụng sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobbies </t>
+  </si>
+  <si>
+    <t>Sử dụng trong gia đình</t>
+  </si>
+  <si>
+    <t>thương hiệu Medela</t>
+  </si>
+  <si>
+    <t>0904187093, 0984898000</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Vân</t>
+  </si>
+  <si>
+    <t>Trang</t>
+  </si>
+  <si>
+    <t>park 11 times city; 362 phố Huế</t>
+  </si>
+  <si>
+    <t>15 dãy 16a7 làng việt kiều châu âu, mộ lao, hà đông;  12 chùa bộc ; 36 ngõ 442 ngách 442/15/28 vĩnh hưng</t>
+  </si>
+  <si>
+    <t>0936875999, 0943579681, 0988928512</t>
+  </si>
+  <si>
+    <t>Cần thông tin chi tiết của sản phẩm</t>
+  </si>
+  <si>
+    <t>xe đẩy, ghế ăn em bé</t>
+  </si>
+  <si>
+    <t>màu hồng</t>
   </si>
 </sst>
 </file>
@@ -2732,7 +2780,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2750,6 +2798,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3055,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G248"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E180" sqref="E180"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7353,8 +7403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G703"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7710,7 +7760,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>936875999</v>
       </c>
@@ -7843,7 +7893,7 @@
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>258</v>
       </c>
@@ -8280,7 +8330,7 @@
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -8664,7 +8714,7 @@
       </c>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>23</v>
       </c>
@@ -8858,7 +8908,7 @@
       </c>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>236</v>
       </c>
@@ -9192,7 +9242,7 @@
       </c>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>23</v>
       </c>
@@ -9232,7 +9282,7 @@
       </c>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>323</v>
       </c>
@@ -10389,7 +10439,7 @@
       </c>
       <c r="G159" s="1"/>
     </row>
-    <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>236</v>
       </c>
@@ -20705,43 +20755,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C02EDA-1C6E-4F46-A0AA-0C36C898044D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C1" t="s">
         <v>839</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>843</v>
+      </c>
+      <c r="E1" t="s">
         <v>840</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>841</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>837</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>851</v>
+      </c>
+      <c r="C2" t="s">
+        <v>853</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>849</v>
+      </c>
+      <c r="E2" t="s">
+        <v>845</v>
+      </c>
+      <c r="F2" t="s">
+        <v>844</v>
+      </c>
+      <c r="G2" t="s">
+        <v>847</v>
+      </c>
+      <c r="H2" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>838</v>
+      </c>
+      <c r="B3" t="s">
+        <v>852</v>
+      </c>
+      <c r="C3" t="s">
+        <v>854</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="E3" t="s">
+        <v>856</v>
+      </c>
+      <c r="F3" t="s">
+        <v>857</v>
+      </c>
+      <c r="G3" t="s">
+        <v>847</v>
+      </c>
+      <c r="H3" t="s">
+        <v>858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>